<commit_message>
New Work organization v2
</commit_message>
<xml_diff>
--- a/data/xlsx/ner_tag.xlsx
+++ b/data/xlsx/ner_tag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFM_Project\PLN_Project\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD0C7B7-415B-47C7-AEE4-75F2621550AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BEB834-ABEF-4750-98D6-752B9E883AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2250" windowWidth="21600" windowHeight="13305" xr2:uid="{5046557F-30AB-4FF6-A1FA-27FE8137B2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5046557F-30AB-4FF6-A1FA-27FE8137B2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="tag" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>tag</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>OTH</t>
+  </si>
+  <si>
+    <t>Otros</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J14:J15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,10 +775,10 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>